<commit_message>
Minor edits in testdata, updated TestNG to 7.0.0
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t xml:space="preserve">title</t>
   </si>
@@ -45,7 +45,7 @@
     <t xml:space="preserve">Bolkonsky</t>
   </si>
   <si>
-    <t xml:space="preserve">Google</t>
+    <t xml:space="preserve">Tolstoy Inc</t>
   </si>
   <si>
     <t xml:space="preserve">Dr.</t>
@@ -57,7 +57,7 @@
     <t xml:space="preserve">Gray</t>
   </si>
   <si>
-    <t xml:space="preserve">Amazon</t>
+    <t xml:space="preserve">Wild LLC</t>
   </si>
   <si>
     <t xml:space="preserve">Mrs.</t>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t xml:space="preserve">Rostova</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ebay</t>
   </si>
 </sst>
 </file>
@@ -192,10 +189,10 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.38671875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -250,7 +247,7 @@
         <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -275,7 +272,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.38671875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -298,7 +295,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.38671875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>